<commit_message>
updated: strategy and command interconnection
</commit_message>
<xml_diff>
--- a/docs/Tasks.xlsx
+++ b/docs/Tasks.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Study Materials\Advanced Software Development\Check-In-Check-out-Framework\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Masters\Advanced Software Development\Labs\Project\Check-In-Check-out-Framework\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>Assignee</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>Logger - Console, File, Db</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -174,8 +177,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -450,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -464,7 +495,7 @@
     <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -481,7 +512,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -497,8 +528,11 @@
       <c r="E2" s="3">
         <v>42561</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -515,7 +549,7 @@
         <v>42561</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -532,7 +566,7 @@
         <v>42561</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -549,7 +583,7 @@
         <v>42561</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -566,7 +600,7 @@
         <v>42562</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -583,7 +617,7 @@
         <v>42563</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -600,7 +634,7 @@
         <v>42564</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -617,7 +651,7 @@
         <v>42565</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -634,7 +668,7 @@
         <v>42566</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>

</xml_diff>